<commit_message>
last diary updated --Weihuan Fu
</commit_message>
<xml_diff>
--- a/diaries/diary-weihuan-fu.xlsx
+++ b/diaries/diary-weihuan-fu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Desktop/SWE-265P/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C165712E-0974-6148-B644-AE00BC3CD8B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C045522-3694-45FA-ADD3-55240EAC5E17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="143">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -393,6 +393,88 @@
   </si>
   <si>
     <t>Amazed by how elegant those design patterns are and ready to learn more about it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn more about key expert practice and get feedback regarding pull request </t>
+  </si>
+  <si>
+    <t>Learn about mechanism for code understanding through reading testing cases</t>
+  </si>
+  <si>
+    <t>Simply reading test cases can help us understand a lot more about the system the test case is aiming for. For deeper understanding, trying to write test cases ourselves can really help us understand how this feature really works in the system. Apart from reading and writing test cases, for smaller projects, I would use other tactics such as print statement or loggings to see what is really happening in the code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feel good that stuff learned from other class (testing class) can be applied to this class. </t>
+  </si>
+  <si>
+    <t>1:00 - 4:00</t>
+  </si>
+  <si>
+    <t>teammates (online)</t>
+  </si>
+  <si>
+    <t>study existing test cases of Cassandra</t>
+  </si>
+  <si>
+    <t>Scanned through almost all test cases and found several interesting ones.</t>
+  </si>
+  <si>
+    <t>We feel it was almost impossible to understand all test cases of Cassandra, just like we can not understand all source code. However, by reading through test cases, we are more clear about how the some feature actually works. We gain better understanding of Cassandra by reading testing codes.</t>
+  </si>
+  <si>
+    <t>Always feel good when learned more but still worried about the last pull request.</t>
+  </si>
+  <si>
+    <t>wrap-up of class</t>
+  </si>
+  <si>
+    <t>reviewed stuff we learned through the quarter especially key expert practice and got a lot of useful advice for my coding career</t>
+  </si>
+  <si>
+    <t>Before this class I realize that as a programmer we should spend most of my time writing code. However, my perspective has changed after a quarter of this class material and all the guest speaking. I realize that even professionals spend a lot of time reading either their own or other's code for different reasons. I do not try to avoid reading code now but instead I choose to read and learn from the code.</t>
+  </si>
+  <si>
+    <t>Feel really good about how to really become an expert in coding</t>
+  </si>
+  <si>
+    <t>work on last pull request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our pull request got approved by Kaj, which means we can really work on it now </t>
+  </si>
+  <si>
+    <t>Finding a pull request that we can actually work on is not too hard (as we only understand part of the whole system, there are limited choices for us)</t>
+  </si>
+  <si>
+    <t>feel good that our pull request got approved, but also worried if we can actually fix that issue.</t>
+  </si>
+  <si>
+    <t>7:00 pm - 12:00</t>
+  </si>
+  <si>
+    <t>Tianyu Qi (online)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feel worried not being able to finish it all. </t>
+  </si>
+  <si>
+    <t>The seemingly straightforward issue can really involved a bunch of code. While trying to fix the pull request, we realize that there are more than 20 files/methods we need to change. Also from the previous research, it seems like only a few out of hundreds of pull requests got merged, however, this is still a good practice for us even we do not expect developers to merge our changes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:00 pm - 9:00 </t>
+  </si>
+  <si>
+    <t>while still working on the last pull request, we  wrote report on our experience for the last homework.</t>
+  </si>
+  <si>
+    <t>feel excited about not having to take the test. Ready to work on the pull request and try to fix issue even after the quarter ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While reading the source code, I was happy to see some design pattern that I recently just learned about. Again design pattern is something that is really important when reading people's code or write my own code in an elegant way.
+</t>
+  </si>
+  <si>
+    <t>finshed part of the fix and there are so much more to do. Wrote a new test case.</t>
   </si>
 </sst>
 </file>
@@ -913,23 +995,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="21.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -940,7 +1022,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -949,7 +1031,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -958,7 +1040,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -971,7 +1053,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -984,7 +1066,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -997,7 +1079,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1006,7 +1088,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1015,7 +1097,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1038,7 +1120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43839</v>
       </c>
@@ -1061,7 +1143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43842</v>
       </c>
@@ -1084,7 +1166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43846</v>
       </c>
@@ -1107,7 +1189,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43850</v>
       </c>
@@ -1130,7 +1212,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43853</v>
       </c>
@@ -1153,7 +1235,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="98" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43858</v>
       </c>
@@ -1176,7 +1258,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="146.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43860</v>
       </c>
@@ -1199,7 +1281,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="146.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43863</v>
       </c>
@@ -1222,7 +1304,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43864</v>
       </c>
@@ -1245,7 +1327,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43866</v>
       </c>
@@ -1268,7 +1350,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43867</v>
       </c>
@@ -1291,7 +1373,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43870</v>
       </c>
@@ -1314,7 +1396,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43877</v>
       </c>
@@ -1337,7 +1419,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="119.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43881</v>
       </c>
@@ -1360,7 +1442,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="176.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43883</v>
       </c>
@@ -1383,7 +1465,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="227" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="227.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43885</v>
       </c>
@@ -1406,7 +1488,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43887</v>
       </c>
@@ -1429,7 +1511,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43888</v>
       </c>
@@ -1452,7 +1534,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="122" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="122.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43891</v>
       </c>
@@ -1475,7 +1557,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43893</v>
       </c>
@@ -1498,61 +1580,145 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>43895</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43897</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>43902</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>43904</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>43905</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>43906</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1561,7 +1727,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1570,7 +1736,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1579,7 +1745,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1588,7 +1754,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1597,7 +1763,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1606,7 +1772,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1615,7 +1781,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1624,7 +1790,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1633,7 +1799,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1642,7 +1808,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1651,7 +1817,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1660,7 +1826,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1669,7 +1835,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1678,7 +1844,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1687,7 +1853,7 @@
       <c r="F50" s="4"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1696,7 +1862,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1705,7 +1871,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1714,7 +1880,7 @@
       <c r="F53" s="4"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1723,7 +1889,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1732,7 +1898,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1741,7 +1907,7 @@
       <c r="F56" s="4"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1750,7 +1916,7 @@
       <c r="F57" s="4"/>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1759,7 +1925,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1768,7 +1934,7 @@
       <c r="F59" s="4"/>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1777,7 +1943,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1786,7 +1952,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1795,7 +1961,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1804,7 +1970,7 @@
       <c r="F63" s="4"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1813,7 +1979,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1822,7 +1988,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1831,7 +1997,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1840,7 +2006,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1849,7 +2015,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1858,7 +2024,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1867,7 +2033,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1876,7 +2042,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1885,7 +2051,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1894,7 +2060,7 @@
       <c r="F73" s="4"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1903,7 +2069,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1912,7 +2078,7 @@
       <c r="F75" s="4"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1921,7 +2087,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1930,7 +2096,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1939,7 +2105,7 @@
       <c r="F78" s="4"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1948,7 +2114,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1957,7 +2123,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1966,7 +2132,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1975,7 +2141,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -1984,7 +2150,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -1993,7 +2159,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -2002,7 +2168,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2011,7 +2177,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -2020,7 +2186,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -2029,7 +2195,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -2038,7 +2204,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -2047,7 +2213,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -2056,7 +2222,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -2065,7 +2231,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -2074,7 +2240,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -2083,7 +2249,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -2092,7 +2258,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -2101,7 +2267,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -2110,7 +2276,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -2119,7 +2285,7 @@
       <c r="F98" s="4"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -2128,7 +2294,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -2137,7 +2303,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -2146,7 +2312,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -2155,7 +2321,7 @@
       <c r="F102" s="4"/>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -2164,7 +2330,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -2173,7 +2339,7 @@
       <c r="F104" s="4"/>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -2182,7 +2348,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -2191,7 +2357,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -2200,7 +2366,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -2209,7 +2375,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -2218,7 +2384,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -2227,7 +2393,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -2236,7 +2402,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -2245,7 +2411,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -2254,7 +2420,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -2263,7 +2429,7 @@
       <c r="F114" s="4"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -2272,7 +2438,7 @@
       <c r="F115" s="4"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
@@ -2281,7 +2447,7 @@
       <c r="F116" s="13"/>
       <c r="G116" s="14"/>
     </row>
-    <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
@@ -2290,7 +2456,7 @@
       <c r="F117" s="13"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
@@ -2299,7 +2465,7 @@
       <c r="F118" s="13"/>
       <c r="G118" s="14"/>
     </row>
-    <row r="119" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
@@ -2308,7 +2474,7 @@
       <c r="F119" s="13"/>
       <c r="G119" s="14"/>
     </row>
-    <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
@@ -2317,7 +2483,7 @@
       <c r="F120" s="13"/>
       <c r="G120" s="14"/>
     </row>
-    <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
@@ -2326,7 +2492,7 @@
       <c r="F121" s="13"/>
       <c r="G121" s="14"/>
     </row>
-    <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
@@ -2335,7 +2501,7 @@
       <c r="F122" s="13"/>
       <c r="G122" s="14"/>
     </row>
-    <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
@@ -2344,7 +2510,7 @@
       <c r="F123" s="13"/>
       <c r="G123" s="14"/>
     </row>
-    <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -2353,7 +2519,7 @@
       <c r="F124" s="13"/>
       <c r="G124" s="14"/>
     </row>
-    <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>
@@ -2362,7 +2528,7 @@
       <c r="F125" s="13"/>
       <c r="G125" s="14"/>
     </row>
-    <row r="126" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
       <c r="B126" s="13"/>
       <c r="C126" s="13"/>

</xml_diff>